<commit_message>
add additional mood input
</commit_message>
<xml_diff>
--- a/Habit Tracker.xlsx
+++ b/Habit Tracker.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qwerty\Desktop\Excel Learning\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB47F594-858E-49B8-8DA4-DA2CC73ED03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921E6811-CC02-4F83-AD9E-B51D9E9DDB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{51730BAA-28DA-4A0A-823D-F90BC72B8190}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51730BAA-28DA-4A0A-823D-F90BC72B8190}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>Categories</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Mood</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -14840,10 +14843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A980A913-6CF3-4DA3-B733-450F2D06DF7B}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15769,6 +15773,99 @@
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>10</v>
+      </c>
+      <c r="S11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T11" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" t="s">
+        <v>10</v>
+      </c>
+      <c r="V11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W11" t="s">
+        <v>10</v>
+      </c>
+      <c r="X11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -15789,7 +15886,7 @@
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:AF11" xr:uid="{F7C8FE0F-85E1-43C3-B73C-1BE8004E4535}">
-      <formula1>"Happy, Neutral, Sad"</formula1>
+      <formula1>"None, Happy, Neutral, Sad"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>